<commit_message>
MN: Proyectos TestNG finales web and mobile
</commit_message>
<xml_diff>
--- a/TestNG/TestNGEjercicioMobile/Data/data.xlsx
+++ b/TestNG/TestNGEjercicioMobile/Data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miltonnino\eclipse-workspace-testNG\TestNGEjercicioMobile\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67E6BB26-23F5-4471-8155-B1278F8C2C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0CBA064-16DF-4F71-AB9F-0B05908E6280}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="calculadora" sheetId="7" r:id="rId1"/>
@@ -485,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02684DB6-1ECC-4ACD-B5E0-B95D95C1EEFA}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -756,7 +756,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F2" t="s">
         <v>28</v>
@@ -801,7 +801,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{186E7C2B-E096-491C-9DDE-9ED4A78FB7A2}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>